<commit_message>
added filled out json files for student&class data
</commit_message>
<xml_diff>
--- a/UniData/StudentData.xlsx
+++ b/UniData/StudentData.xlsx
@@ -5,27 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc0505c6d357893e/Desktop/Universal Storage Unit/Code/Godot 4 Projects/Registraren't/StudentData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc0505c6d357893e/Desktop/Universal Storage Unit/Code/Godot 4 Projects/Registraren't/UniData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="11_F25DC773A252ABDACC104816B9DF49C85ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5BAC5EA-D447-4156-82FB-5566FDEE8876}"/>
+  <xr:revisionPtr revIDLastSave="198" documentId="11_F25DC773A252ABDACC104816B9DF49C85ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C97A6D5-E375-4FC9-B71A-89E357C67BFB}"/>
   <bookViews>
-    <workbookView xWindow="29565" yWindow="4080" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4530" yWindow="2505" windowWidth="23265" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -60,27 +71,21 @@
     <t>Friday</t>
   </si>
   <si>
+    <t>Sophomore</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>Good</t>
   </si>
   <si>
-    <t>Bob Smith</t>
-  </si>
-  <si>
-    <t>Sophomore</t>
-  </si>
-  <si>
-    <t>Computer Science</t>
-  </si>
-  <si>
-    <t>Art</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Jane Doe</t>
-  </si>
-  <si>
     <t>Freshman</t>
   </si>
   <si>
@@ -93,10 +98,109 @@
     <t>Delinquent</t>
   </si>
   <si>
-    <t xml:space="preserve">CS 101, EN 133, ART 222 </t>
-  </si>
-  <si>
-    <t>ART 222</t>
+    <t xml:space="preserve">CS 101,EN 133,ART 222 </t>
+  </si>
+  <si>
+    <t>Conor Schultz</t>
+  </si>
+  <si>
+    <t>Marco Cardenas</t>
+  </si>
+  <si>
+    <t>Christopher Singh</t>
+  </si>
+  <si>
+    <t>Dominik Gamble</t>
+  </si>
+  <si>
+    <t>Joe Gibbs</t>
+  </si>
+  <si>
+    <t>Alana Wright</t>
+  </si>
+  <si>
+    <t>Richard Hendricks</t>
+  </si>
+  <si>
+    <t>Thomas Chen</t>
+  </si>
+  <si>
+    <t>Jorge Irwin</t>
+  </si>
+  <si>
+    <t>Senior</t>
+  </si>
+  <si>
+    <t>Junior</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Political Science</t>
+  </si>
+  <si>
+    <t>CS 213,MAT 218</t>
+  </si>
+  <si>
+    <t>CS 101,EN 133,CS 213D</t>
+  </si>
+  <si>
+    <t>ART 101,ART 115</t>
+  </si>
+  <si>
+    <t>MAT 206,EN 204</t>
+  </si>
+  <si>
+    <t>ART 320,AHIS 319</t>
+  </si>
+  <si>
+    <t>ART 441,AHIS 333</t>
+  </si>
+  <si>
+    <t>EN 133,ART 115</t>
+  </si>
+  <si>
+    <t>EN 168,ART 177</t>
+  </si>
+  <si>
+    <t>EN 168</t>
+  </si>
+  <si>
+    <t>EN 133,AHIS 110A,AHIS 110B</t>
+  </si>
+  <si>
+    <t>POLS 201,POLS 225,EN 211</t>
+  </si>
+  <si>
+    <t>EN 218,EN 204</t>
+  </si>
+  <si>
+    <t>MAT 218,MAT 220</t>
+  </si>
+  <si>
+    <t>CS 202,CS 213,CS 213D</t>
+  </si>
+  <si>
+    <t>CS 405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CS 405 </t>
+  </si>
+  <si>
+    <t>MAT 337,MAT 359</t>
+  </si>
+  <si>
+    <t>CS 318,CS 312,AHIS 319</t>
+  </si>
+  <si>
+    <t>AHIS 214,AHIS 255</t>
   </si>
 </sst>
 </file>
@@ -418,17 +522,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -468,48 +580,317 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>